<commit_message>
added color coding for values
</commit_message>
<xml_diff>
--- a/Report.xlsx
+++ b/Report.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="74">
   <si>
     <t>NUME</t>
   </si>
@@ -36,196 +36,205 @@
     <t>Nu a fost gasit in excel</t>
   </si>
   <si>
+    <t>Telefon mobil Apple iPhone 14 Pro, 128GB, 5G, Space Black</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 14, 128GB, 5G, Starlight</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 14 Pro Max, 128GB, 5G, Space Black</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 14, 128GB, 5G, Midnight</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 14 Pro, 128GB, 5G, Deep Purple</t>
+  </si>
+  <si>
+    <t>6.339,99 Lei</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 11, 64GB, White</t>
+  </si>
+  <si>
+    <t>2.399,99 Lei</t>
+  </si>
+  <si>
+    <t>2.199,99 Lei</t>
+  </si>
+  <si>
+    <t>200.0</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 14, 128GB, 5G, Purple</t>
+  </si>
+  <si>
     <t>Telefon mobil Apple iPhone 13, 128GB, 5G, Midnight</t>
   </si>
   <si>
-    <t>3.999,99 Lei</t>
+    <t>3.899,99 Lei</t>
   </si>
   <si>
     <t>4.099,99 Lei</t>
   </si>
   <si>
-    <t>-100.0</t>
+    <t>-200.0</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 14 Pro Max, 128GB, 5G, Deep Purple</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 14 Pro Max, 256GB, 5G, Deep Purple</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 14 Pro, 256GB, 5G, Space Black</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 12 mini, 128GB, 5G, White</t>
   </si>
   <si>
     <t>Telefon mobil Apple iPhone 11, 128GB, Black</t>
   </si>
   <si>
-    <t>Telefon mobil Apple iPhone 14 Pro, 128GB, 5G, Space Black</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 14 Pro, 128GB, 5G, Deep Purple</t>
-  </si>
-  <si>
-    <t>6.339,99 Lei</t>
-  </si>
-  <si>
-    <t>0.0</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 14, 128GB, 5G, Purple</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 14 Pro Max, 128GB, 5G, Space Black</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 14, 128GB, 5G, Midnight</t>
+    <t>Telefon mobil Apple iPhone 14 Pro Max, 256GB, 5G, Space Black</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 11, 64GB, Black</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 14 Pro, 256GB, 5G, Deep Purple</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 14 Plus, 128GB, 5G, Purple</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 14 Pro Max, 128GB, 5G, Gold</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 13, 128GB, 5G, Pink</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 14 Plus, 128GB, 5G, Blue</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 14 Plus, 128GB, 5G, Starlight</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 14, 256GB, 5G, Midnight</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 14 Pro, 128GB, 5G, Silver</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 14, 256GB, 5G, Starlight</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 14 Pro Max, 128GB, 5G, Silver</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 14 Pro, 128GB, 5G, Gold</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 14 Pro Max, 256GB, 5G, Gold</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 14, 256GB, 5G, Blue</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 13, 128GB, 5G, Starlight</t>
   </si>
   <si>
     <t>Telefon mobil Apple iPhone 13, 128GB, 5G, Blue</t>
   </si>
   <si>
-    <t>Telefon mobil Apple iPhone 14, 128GB, 5G, Starlight</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 11, 64GB, White</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 14 Pro Max, 128GB, 5G, Gold</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 14 Pro Max, 128GB, 5G, Deep Purple</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 14 Pro, 256GB, 5G, Deep Purple</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 14 Pro Max, 256GB, 5G, Space Black</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 14 Pro Max, 256GB, 5G, Deep Purple</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 11, 64GB, Black</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 14 Pro, 256GB, 5G, Space Black</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 14 Plus, 128GB, 5G, Blue</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 14 Pro Max, 256GB, 5G, Gold</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 13, 128GB, 5G, Pink</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 12 mini, 128GB, 5G, Blue</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 14 Pro, 128GB, 5G, Silver</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 14 Pro Max, 128GB, 5G, Silver</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 14 Pro, 128GB, 5G, Gold</t>
+    <t>Telefon mobil Apple iPhone 14 Pro Max, 1TB, 5G, Space Black</t>
   </si>
   <si>
     <t>Telefon mobil Apple iPhone 14 Pro Max, 1TB, 5G, Deep Purple</t>
   </si>
   <si>
-    <t>Telefon mobil Apple iPhone 12 mini, 128GB, 5G, White</t>
+    <t>Telefon mobil Apple iPhone 14 Plus, 128GB, 5G, Midnight</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 14 Pro, 256GB, 5G, Gold</t>
   </si>
   <si>
     <t>Telefon mobil Apple iPhone 14 Pro Max, 256GB, 5G, Silver</t>
   </si>
   <si>
-    <t>Telefon mobil Apple iPhone 13, 128GB, 5G, Starlight</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 14 Plus, 128GB, 5G, Midnight</t>
+    <t>Telefon mobil Apple iPhone 14, 256GB, 5G, RED</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 11, 128GB, White</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 13 mini, 128GB, 5G, Midnight</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 14, 128GB, 5G, RED</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 14 Plus, 256GB, 5G, Midnight</t>
   </si>
   <si>
     <t>Telefon mobil Apple iPhone 13, 128GB, 5G, Green</t>
   </si>
   <si>
-    <t>Telefon mobil Apple iPhone 14 Pro, 256GB, 5G, Gold</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 14 Plus, 128GB, 5G, Starlight</t>
+    <t>Telefon mobil Apple iPhone 12, 128GB, 5G, Black</t>
   </si>
   <si>
     <t>Telefon mobil Apple iPhone 14 Pro Max, 1TB, 5G, Gold</t>
   </si>
   <si>
-    <t>Telefon mobil Apple iPhone 14, 256GB, 5G, Starlight</t>
+    <t>Telefon mobil Apple iPhone 14, 256GB, 5G, Purple</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 14 Pro Max, 512GB, 5G, Deep Purple</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 13, 128GB, 5G, Red</t>
   </si>
   <si>
     <t>Telefon mobil Apple iPhone 14 Pro, 256GB, 5G, Silver</t>
   </si>
   <si>
-    <t>Telefon mobil Apple iPhone 14, 128GB, 5G, RED</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 12, 128GB, 5G, Black</t>
-  </si>
-  <si>
     <t>Telefon mobil Apple iPhone 13 mini, 128GB, 5G, Starlight</t>
   </si>
   <si>
-    <t>Telefon mobil Apple iPhone 11, 128GB, White</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 14, 256GB, 5G, Blue</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 14 Pro Max, 1TB, 5G, Space Black</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 14 Plus, 256GB, 5G, Midnight</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 12, 128GB, 5G, Blue</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 14 Plus, 128GB, 5G, Purple</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 14, 256GB, 5G, Midnight</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 14, 256GB, 5G, Purple</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 13 mini, 128GB, 5G, Midnight</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 12, 64GB, 5G, Black</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 13 Pro, 128GB, 5G, Sierra Blue</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 13, 128GB, 5G, Red</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 14 Pro Max, 512GB, 5G, Deep Purple</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 8, 64GB, 4G, Space Grey</t>
+    <t>Telefon mobil Apple iPhone 13 mini, 128GB, 5G, Pink</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 12, 128GB, 5G, (PRODUCT)RED</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 14 Plus, 128GB, 5G, RED</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 12, 128GB, 5G, White</t>
   </si>
   <si>
     <t>Telefon mobil Apple iPhone 13, 256GB, 5G, Midnight</t>
   </si>
   <si>
-    <t>Telefon mobil Apple iPhone XS, 64GB, Space Grey</t>
+    <t>Telefon mobil Apple iPhone 14 Pro Max, 1TB, 5G, Silver</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 13, 256GB, 5G, Blue</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 13, 256GB, 5G, Pink</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 13, 256GB, 5G, Green</t>
+  </si>
+  <si>
+    <t>Telefon mobil Apple iPhone 14 Pro Max, 512GB, 5G, Gold</t>
   </si>
   <si>
     <t>Telefon mobil Apple iPhone 14 Pro Max, 512GB, 5G, Space Black</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 13 mini, 128GB, 5G, Pink</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 14 Plus, 128GB, 5G, RED</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 8, 64GB, 4G, Gold</t>
-  </si>
-  <si>
-    <t>Telefon mobil Apple iPhone 12, 64GB, 5G, Blue</t>
   </si>
 </sst>
 </file>
@@ -247,12 +256,42 @@
       <b val="true"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="darkGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="12"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightTrellis">
+        <bgColor indexed="12"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightTrellis">
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightTrellis">
+        <bgColor indexed="10"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -267,16 +306,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -304,33 +346,47 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4"/>
+        <v>16</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -338,7 +394,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B119"/>
+  <dimension ref="A1:B178"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -374,7 +430,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -382,7 +438,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -390,7 +446,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -398,7 +454,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -406,7 +462,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -414,7 +470,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -422,7 +478,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -430,7 +486,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -438,7 +494,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -446,7 +502,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -454,7 +510,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -462,7 +518,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
@@ -470,7 +526,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -478,7 +534,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -486,7 +542,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -494,7 +550,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
@@ -502,7 +558,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
@@ -510,7 +566,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
@@ -518,7 +574,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
@@ -526,7 +582,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
         <v>6</v>
@@ -534,7 +590,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
         <v>6</v>
@@ -542,7 +598,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B25" t="s">
         <v>6</v>
@@ -550,7 +606,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
         <v>6</v>
@@ -558,7 +614,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27" t="s">
         <v>6</v>
@@ -566,7 +622,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B28" t="s">
         <v>6</v>
@@ -574,7 +630,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B29" t="s">
         <v>6</v>
@@ -582,7 +638,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B30" t="s">
         <v>6</v>
@@ -590,7 +646,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B31" t="s">
         <v>6</v>
@@ -598,7 +654,7 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
@@ -606,7 +662,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B33" t="s">
         <v>6</v>
@@ -614,7 +670,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B34" t="s">
         <v>6</v>
@@ -622,7 +678,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B35" t="s">
         <v>6</v>
@@ -630,7 +686,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B36" t="s">
         <v>6</v>
@@ -638,7 +694,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B37" t="s">
         <v>6</v>
@@ -646,7 +702,7 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B38" t="s">
         <v>6</v>
@@ -654,7 +710,7 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B39" t="s">
         <v>6</v>
@@ -662,7 +718,7 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B40" t="s">
         <v>6</v>
@@ -670,7 +726,7 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B41" t="s">
         <v>6</v>
@@ -678,7 +734,7 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B42" t="s">
         <v>6</v>
@@ -686,7 +742,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B43" t="s">
         <v>6</v>
@@ -694,7 +750,7 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B44" t="s">
         <v>6</v>
@@ -702,7 +758,7 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B45" t="s">
         <v>6</v>
@@ -710,7 +766,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B46" t="s">
         <v>6</v>
@@ -718,7 +774,7 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B47" t="s">
         <v>6</v>
@@ -726,7 +782,7 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B48" t="s">
         <v>6</v>
@@ -734,7 +790,7 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B49" t="s">
         <v>6</v>
@@ -742,7 +798,7 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B50" t="s">
         <v>6</v>
@@ -750,7 +806,7 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B51" t="s">
         <v>6</v>
@@ -758,7 +814,7 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B52" t="s">
         <v>6</v>
@@ -766,7 +822,7 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B53" t="s">
         <v>6</v>
@@ -774,7 +830,7 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B54" t="s">
         <v>6</v>
@@ -782,7 +838,7 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B55" t="s">
         <v>6</v>
@@ -790,7 +846,7 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B56" t="s">
         <v>6</v>
@@ -798,7 +854,7 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B57" t="s">
         <v>6</v>
@@ -806,7 +862,7 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B58" t="s">
         <v>6</v>
@@ -814,7 +870,7 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B59" t="s">
         <v>6</v>
@@ -822,7 +878,7 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B60" t="s">
         <v>6</v>
@@ -830,7 +886,7 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B61" t="s">
         <v>6</v>
@@ -838,7 +894,7 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B62" t="s">
         <v>6</v>
@@ -846,7 +902,7 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B63" t="s">
         <v>6</v>
@@ -854,7 +910,7 @@
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B64" t="s">
         <v>6</v>
@@ -862,7 +918,7 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B65" t="s">
         <v>6</v>
@@ -870,7 +926,7 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B66" t="s">
         <v>6</v>
@@ -878,7 +934,7 @@
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B67" t="s">
         <v>6</v>
@@ -886,7 +942,7 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B68" t="s">
         <v>6</v>
@@ -894,7 +950,7 @@
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B69" t="s">
         <v>6</v>
@@ -902,7 +958,7 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B70" t="s">
         <v>6</v>
@@ -910,7 +966,7 @@
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B71" t="s">
         <v>6</v>
@@ -918,7 +974,7 @@
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B72" t="s">
         <v>6</v>
@@ -926,7 +982,7 @@
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B73" t="s">
         <v>6</v>
@@ -934,7 +990,7 @@
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B74" t="s">
         <v>6</v>
@@ -942,7 +998,7 @@
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B75" t="s">
         <v>6</v>
@@ -950,7 +1006,7 @@
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B76" t="s">
         <v>6</v>
@@ -958,7 +1014,7 @@
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B77" t="s">
         <v>6</v>
@@ -966,7 +1022,7 @@
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B78" t="s">
         <v>6</v>
@@ -974,7 +1030,7 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B79" t="s">
         <v>6</v>
@@ -982,7 +1038,7 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B80" t="s">
         <v>6</v>
@@ -990,7 +1046,7 @@
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B81" t="s">
         <v>6</v>
@@ -998,7 +1054,7 @@
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B82" t="s">
         <v>6</v>
@@ -1006,7 +1062,7 @@
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B83" t="s">
         <v>6</v>
@@ -1014,7 +1070,7 @@
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B84" t="s">
         <v>6</v>
@@ -1022,7 +1078,7 @@
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B85" t="s">
         <v>6</v>
@@ -1030,7 +1086,7 @@
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B86" t="s">
         <v>6</v>
@@ -1038,7 +1094,7 @@
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B87" t="s">
         <v>6</v>
@@ -1046,7 +1102,7 @@
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B88" t="s">
         <v>6</v>
@@ -1054,7 +1110,7 @@
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B89" t="s">
         <v>6</v>
@@ -1062,7 +1118,7 @@
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B90" t="s">
         <v>6</v>
@@ -1070,7 +1126,7 @@
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B91" t="s">
         <v>6</v>
@@ -1078,7 +1134,7 @@
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B92" t="s">
         <v>6</v>
@@ -1086,7 +1142,7 @@
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B93" t="s">
         <v>6</v>
@@ -1094,7 +1150,7 @@
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B94" t="s">
         <v>6</v>
@@ -1102,7 +1158,7 @@
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B95" t="s">
         <v>6</v>
@@ -1110,7 +1166,7 @@
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B96" t="s">
         <v>6</v>
@@ -1118,7 +1174,7 @@
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B97" t="s">
         <v>6</v>
@@ -1126,7 +1182,7 @@
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B98" t="s">
         <v>6</v>
@@ -1134,7 +1190,7 @@
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B99" t="s">
         <v>6</v>
@@ -1142,7 +1198,7 @@
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="B100" t="s">
         <v>6</v>
@@ -1150,7 +1206,7 @@
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B101" t="s">
         <v>6</v>
@@ -1158,7 +1214,7 @@
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="B102" t="s">
         <v>6</v>
@@ -1166,7 +1222,7 @@
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="B103" t="s">
         <v>6</v>
@@ -1174,7 +1230,7 @@
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="B104" t="s">
         <v>6</v>
@@ -1182,7 +1238,7 @@
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="B105" t="s">
         <v>6</v>
@@ -1190,7 +1246,7 @@
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="B106" t="s">
         <v>6</v>
@@ -1198,7 +1254,7 @@
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B107" t="s">
         <v>6</v>
@@ -1206,7 +1262,7 @@
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="B108" t="s">
         <v>6</v>
@@ -1214,7 +1270,7 @@
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="B109" t="s">
         <v>6</v>
@@ -1222,7 +1278,7 @@
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="B110" t="s">
         <v>6</v>
@@ -1230,7 +1286,7 @@
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="B111" t="s">
         <v>6</v>
@@ -1238,7 +1294,7 @@
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="B112" t="s">
         <v>6</v>
@@ -1246,7 +1302,7 @@
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B113" t="s">
         <v>6</v>
@@ -1254,7 +1310,7 @@
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="B114" t="s">
         <v>6</v>
@@ -1262,7 +1318,7 @@
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="B115" t="s">
         <v>6</v>
@@ -1270,7 +1326,7 @@
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="B116" t="s">
         <v>6</v>
@@ -1278,7 +1334,7 @@
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="B117" t="s">
         <v>6</v>
@@ -1286,7 +1342,7 @@
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="B118" t="s">
         <v>6</v>
@@ -1294,9 +1350,481 @@
     </row>
     <row r="119">
       <c r="A119" t="s">
+        <v>54</v>
+      </c>
+      <c r="B119" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s">
+        <v>54</v>
+      </c>
+      <c r="B120" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="s">
+        <v>54</v>
+      </c>
+      <c r="B121" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="s">
+        <v>55</v>
+      </c>
+      <c r="B122" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s">
+        <v>55</v>
+      </c>
+      <c r="B123" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s">
+        <v>55</v>
+      </c>
+      <c r="B124" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s">
+        <v>56</v>
+      </c>
+      <c r="B125" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s">
+        <v>56</v>
+      </c>
+      <c r="B126" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s">
+        <v>56</v>
+      </c>
+      <c r="B127" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s">
+        <v>57</v>
+      </c>
+      <c r="B128" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s">
+        <v>57</v>
+      </c>
+      <c r="B129" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s">
+        <v>57</v>
+      </c>
+      <c r="B130" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s">
+        <v>58</v>
+      </c>
+      <c r="B131" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s">
+        <v>58</v>
+      </c>
+      <c r="B132" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="s">
+        <v>58</v>
+      </c>
+      <c r="B133" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="s">
+        <v>59</v>
+      </c>
+      <c r="B134" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s">
+        <v>59</v>
+      </c>
+      <c r="B135" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s">
+        <v>59</v>
+      </c>
+      <c r="B136" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="s">
+        <v>60</v>
+      </c>
+      <c r="B137" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="s">
+        <v>60</v>
+      </c>
+      <c r="B138" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="s">
+        <v>60</v>
+      </c>
+      <c r="B139" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="s">
+        <v>61</v>
+      </c>
+      <c r="B140" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="s">
+        <v>61</v>
+      </c>
+      <c r="B141" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="s">
+        <v>61</v>
+      </c>
+      <c r="B142" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="s">
+        <v>62</v>
+      </c>
+      <c r="B143" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="s">
+        <v>62</v>
+      </c>
+      <c r="B144" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="s">
+        <v>62</v>
+      </c>
+      <c r="B145" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s">
+        <v>63</v>
+      </c>
+      <c r="B146" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s">
+        <v>63</v>
+      </c>
+      <c r="B147" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s">
+        <v>63</v>
+      </c>
+      <c r="B148" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s">
+        <v>64</v>
+      </c>
+      <c r="B149" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="s">
+        <v>64</v>
+      </c>
+      <c r="B150" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="s">
+        <v>64</v>
+      </c>
+      <c r="B151" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="s">
+        <v>65</v>
+      </c>
+      <c r="B152" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="s">
+        <v>65</v>
+      </c>
+      <c r="B153" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="s">
+        <v>65</v>
+      </c>
+      <c r="B154" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="s">
+        <v>66</v>
+      </c>
+      <c r="B155" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="s">
+        <v>66</v>
+      </c>
+      <c r="B156" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="s">
+        <v>66</v>
+      </c>
+      <c r="B157" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="s">
+        <v>67</v>
+      </c>
+      <c r="B158" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="s">
+        <v>67</v>
+      </c>
+      <c r="B159" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="s">
+        <v>67</v>
+      </c>
+      <c r="B160" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="s">
+        <v>68</v>
+      </c>
+      <c r="B161" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="s">
+        <v>68</v>
+      </c>
+      <c r="B162" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="s">
+        <v>68</v>
+      </c>
+      <c r="B163" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="s">
+        <v>69</v>
+      </c>
+      <c r="B164" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="s">
+        <v>69</v>
+      </c>
+      <c r="B165" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="s">
+        <v>69</v>
+      </c>
+      <c r="B166" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="s">
         <v>70</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B167" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="s">
+        <v>70</v>
+      </c>
+      <c r="B168" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="s">
+        <v>70</v>
+      </c>
+      <c r="B169" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="s">
+        <v>71</v>
+      </c>
+      <c r="B170" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="s">
+        <v>71</v>
+      </c>
+      <c r="B171" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="s">
+        <v>71</v>
+      </c>
+      <c r="B172" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="s">
+        <v>72</v>
+      </c>
+      <c r="B173" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="s">
+        <v>72</v>
+      </c>
+      <c r="B174" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="s">
+        <v>72</v>
+      </c>
+      <c r="B175" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="s">
+        <v>73</v>
+      </c>
+      <c r="B176" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="s">
+        <v>73</v>
+      </c>
+      <c r="B177" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="s">
+        <v>73</v>
+      </c>
+      <c r="B178" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>